<commit_message>
Blacklitterman & expectations inclusion
</commit_message>
<xml_diff>
--- a/AdministracionDePortafolios/166504.xlsx
+++ b/AdministracionDePortafolios/166504.xlsx
@@ -5,174 +5,175 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laygr/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laygr/Documents/Visual Studio 2017/Projects/AdministracionDePortafolios/AdministracionDePortafolios/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="1140" windowWidth="23380" windowHeight="16680" activeTab="2"/>
+    <workbookView xWindow="20" yWindow="1140" windowWidth="23380" windowHeight="16680" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
     <sheet name="Cutoff" sheetId="2" r:id="rId2"/>
     <sheet name="Por utilidad" sheetId="4" r:id="rId3"/>
-    <sheet name="Omega" sheetId="5" r:id="rId4"/>
-    <sheet name="ExpectedReturns" sheetId="6" r:id="rId5"/>
-    <sheet name="óptimo Mínima Varianza" sheetId="3" r:id="rId6"/>
+    <sheet name="BenchmarkWeights" sheetId="7" r:id="rId4"/>
+    <sheet name="Omega" sheetId="5" r:id="rId5"/>
+    <sheet name="ExpectedReturns" sheetId="6" r:id="rId6"/>
+    <sheet name="óptimo Mínima Varianza" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$F$11:$Y$11</definedName>
+    <definedName name="solver_adj" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$F$11:$Y$11</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">'Por utilidad'!$F$14:$Y$14</definedName>
-    <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$F$11</definedName>
+    <definedName name="solver_lhs1" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$F$11</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Por utilidad'!$F$14</definedName>
-    <definedName name="solver_lhs10" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$Q$11</definedName>
+    <definedName name="solver_lhs10" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$Q$11</definedName>
     <definedName name="solver_lhs10" localSheetId="2" hidden="1">'Por utilidad'!$Q$14</definedName>
-    <definedName name="solver_lhs11" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$R$11</definedName>
+    <definedName name="solver_lhs11" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$R$11</definedName>
     <definedName name="solver_lhs11" localSheetId="2" hidden="1">'Por utilidad'!$R$14</definedName>
-    <definedName name="solver_lhs12" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$T$11</definedName>
+    <definedName name="solver_lhs12" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$T$11</definedName>
     <definedName name="solver_lhs12" localSheetId="2" hidden="1">'Por utilidad'!$T$14</definedName>
-    <definedName name="solver_lhs13" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$U$11</definedName>
+    <definedName name="solver_lhs13" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$U$11</definedName>
     <definedName name="solver_lhs13" localSheetId="2" hidden="1">'Por utilidad'!$U$14</definedName>
-    <definedName name="solver_lhs14" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$V$11</definedName>
+    <definedName name="solver_lhs14" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$V$11</definedName>
     <definedName name="solver_lhs14" localSheetId="2" hidden="1">'Por utilidad'!$V$14</definedName>
-    <definedName name="solver_lhs15" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$X$11</definedName>
+    <definedName name="solver_lhs15" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$X$11</definedName>
     <definedName name="solver_lhs15" localSheetId="2" hidden="1">'Por utilidad'!$X$14</definedName>
-    <definedName name="solver_lhs16" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$Y$11</definedName>
+    <definedName name="solver_lhs16" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$Y$11</definedName>
     <definedName name="solver_lhs16" localSheetId="2" hidden="1">'Por utilidad'!$Y$14</definedName>
     <definedName name="solver_lhs17" localSheetId="2" hidden="1">'Por utilidad'!$Y$14</definedName>
-    <definedName name="solver_lhs2" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$F$11:$Y$11</definedName>
+    <definedName name="solver_lhs2" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$F$11:$Y$11</definedName>
     <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Por utilidad'!$F$14:$Y$14</definedName>
-    <definedName name="solver_lhs3" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$G$11</definedName>
+    <definedName name="solver_lhs3" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$G$11</definedName>
     <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Por utilidad'!$G$14</definedName>
-    <definedName name="solver_lhs4" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$H$11</definedName>
+    <definedName name="solver_lhs4" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$H$11</definedName>
     <definedName name="solver_lhs4" localSheetId="2" hidden="1">'Por utilidad'!$H$14</definedName>
-    <definedName name="solver_lhs5" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$H$14</definedName>
+    <definedName name="solver_lhs5" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$H$14</definedName>
     <definedName name="solver_lhs5" localSheetId="2" hidden="1">'Por utilidad'!$H$17</definedName>
-    <definedName name="solver_lhs6" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$I$11</definedName>
+    <definedName name="solver_lhs6" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$I$11</definedName>
     <definedName name="solver_lhs6" localSheetId="2" hidden="1">'Por utilidad'!$I$14</definedName>
-    <definedName name="solver_lhs7" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$M$11</definedName>
+    <definedName name="solver_lhs7" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$M$11</definedName>
     <definedName name="solver_lhs7" localSheetId="2" hidden="1">'Por utilidad'!$M$14</definedName>
-    <definedName name="solver_lhs8" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$N$11</definedName>
+    <definedName name="solver_lhs8" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$N$11</definedName>
     <definedName name="solver_lhs8" localSheetId="2" hidden="1">'Por utilidad'!$N$14</definedName>
-    <definedName name="solver_lhs9" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$P$11</definedName>
+    <definedName name="solver_lhs9" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$P$11</definedName>
     <definedName name="solver_lhs9" localSheetId="2" hidden="1">'Por utilidad'!$P$14</definedName>
-    <definedName name="solver_lin" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_lin" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_mip" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="5" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="5" hidden="1">16</definedName>
+    <definedName name="solver_num" localSheetId="6" hidden="1">16</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">16</definedName>
-    <definedName name="solver_opt" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$G$7</definedName>
+    <definedName name="solver_opt" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$G$7</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">'Por utilidad'!$G$10</definedName>
-    <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel10" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel10" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel10" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel11" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel11" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel11" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel12" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel12" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel12" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel13" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel13" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel13" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel14" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel14" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel14" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel15" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel15" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel15" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel16" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel16" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel16" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel17" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel2" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="6" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="solver_rel3" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel4" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel4" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel4" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel5" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel5" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel5" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel6" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel6" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel6" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel7" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel7" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel7" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel8" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel8" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel8" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel9" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel9" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel9" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rhs1" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs1" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rhs10" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs10" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rhs10" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rhs11" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs11" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rhs11" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rhs12" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs12" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rhs12" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rhs13" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs13" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rhs13" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rhs14" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs14" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rhs14" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rhs15" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs15" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rhs15" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rhs16" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs16" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rhs16" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs17" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rhs2" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rhs3" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rhs4" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs4" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rhs5" localSheetId="5" hidden="1">'óptimo Mínima Varianza'!$J$14</definedName>
+    <definedName name="solver_rhs5" localSheetId="6" hidden="1">'óptimo Mínima Varianza'!$J$14</definedName>
     <definedName name="solver_rhs5" localSheetId="2" hidden="1">'Por utilidad'!$J$17</definedName>
-    <definedName name="solver_rhs6" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs6" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rhs6" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rhs7" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs7" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rhs7" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rhs8" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs8" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rhs8" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rhs9" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs9" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rhs9" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="5" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">2</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateDelta="1.0000000000000001E-5" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -5600,7 +5601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:Y50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="75" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -7948,11 +7949,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
     <mergeCell ref="C49:E49"/>
     <mergeCell ref="C50:E50"/>
     <mergeCell ref="B30:E30"/>
@@ -7969,12 +7965,64 @@
     <mergeCell ref="C41:E41"/>
     <mergeCell ref="C42:E42"/>
     <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0.12336215500910586</v>
+      </c>
+      <c r="B1">
+        <v>0.12041894142789623</v>
+      </c>
+      <c r="C1">
+        <v>0.10136925736987466</v>
+      </c>
+      <c r="D1">
+        <v>9.7439695205180976E-2</v>
+      </c>
+      <c r="E1">
+        <v>9.6008811574885555E-2</v>
+      </c>
+      <c r="F1">
+        <v>9.402616461244373E-2</v>
+      </c>
+      <c r="G1">
+        <v>9.329537132136162E-2</v>
+      </c>
+      <c r="H1">
+        <v>9.2591334918565374E-2</v>
+      </c>
+      <c r="I1">
+        <v>9.2014056840512698E-2</v>
+      </c>
+      <c r="J1">
+        <v>8.9474211720173308E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T20"/>
   <sheetViews>
@@ -9229,7 +9277,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1"/>
   <sheetViews>
@@ -9306,7 +9354,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:Y47"/>
   <sheetViews>
@@ -11641,6 +11689,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="C29:E29"/>
@@ -11653,14 +11709,6 @@
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>